<commit_message>
Adding new performance tests result without kubernetes proxy
</commit_message>
<xml_diff>
--- a/JMeter test results/Jmeter performance .xlsx
+++ b/JMeter test results/Jmeter performance .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>MultiThreaded tests</t>
   </si>
@@ -50,7 +50,28 @@
     <t>Readers Throughput with cache (correct reads per second)</t>
   </si>
   <si>
-    <t>Readers Throughput no cache (correct reads per second)</t>
+    <t>JMS</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Active MQ (local)</t>
+  </si>
+  <si>
+    <t>MongoDBP (through cubernetes proxy)</t>
+  </si>
+  <si>
+    <t>MongoDBC (in cubernetes without proxy)</t>
+  </si>
+  <si>
+    <t>MongoDBP Readers Throughput no cache (correct reads per second)</t>
+  </si>
+  <si>
+    <t>MongoDBC Readers Throughput no cache (correct reads per second)</t>
+  </si>
+  <si>
+    <t>Proxy died</t>
   </si>
 </sst>
 </file>
@@ -153,10 +174,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>LazyWriterManyReaders!$B$11:$H$11</c:f>
+              <c:f>LazyWriterManyReaders!$B$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -177,16 +198,22 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LazyWriterManyReaders!$B$12:$H$12</c:f>
+              <c:f>LazyWriterManyReaders!$B$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>1946.2</c:v>
                 </c:pt>
@@ -222,7 +249,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Readers Throughput no cache (correct reads per second)</c:v>
+                  <c:v>MongoDBP Readers Throughput no cache (correct reads per second)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -239,12 +266,48 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>LazyWriterManyReaders!$B$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>LazyWriterManyReaders!$B$13:$H$13</c:f>
+              <c:f>LazyWriterManyReaders!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>320.3</c:v>
                 </c:pt>
@@ -265,6 +328,76 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3262.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4313.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LazyWriterManyReaders!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MongoDBC Readers Throughput no cache (correct reads per second)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>LazyWriterManyReaders!$B$16:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>446.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1057.4000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1542.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2204</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3291</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3430.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4035.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4681.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4996.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,11 +413,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="294318312"/>
-        <c:axId val="294321056"/>
+        <c:axId val="159316568"/>
+        <c:axId val="159754512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="294318312"/>
+        <c:axId val="159316568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -327,7 +460,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294321056"/>
+        <c:crossAx val="159754512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -335,7 +468,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="294321056"/>
+        <c:axId val="159754512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +519,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="294318312"/>
+        <c:crossAx val="159316568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1028,15 +1161,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1321,24 +1454,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:H14"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1354,12 +1511,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1384,8 +1541,14 @@
       <c r="H11">
         <v>50</v>
       </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>200</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1411,9 +1574,9 @@
         <v>16357.4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>320.3</v>
@@ -1436,8 +1599,14 @@
       <c r="H13">
         <v>3262.1</v>
       </c>
+      <c r="I13">
+        <v>4313.3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -1468,6 +1637,38 @@
       <c r="H14">
         <f t="shared" si="0"/>
         <v>5.0143772416541488</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>446.8</v>
+      </c>
+      <c r="C16">
+        <v>1057.4000000000001</v>
+      </c>
+      <c r="D16">
+        <v>1542.1</v>
+      </c>
+      <c r="E16">
+        <v>2204</v>
+      </c>
+      <c r="F16">
+        <v>3291</v>
+      </c>
+      <c r="G16">
+        <v>3430.6</v>
+      </c>
+      <c r="H16">
+        <v>4035.1</v>
+      </c>
+      <c r="I16">
+        <v>4681.3</v>
+      </c>
+      <c r="J16">
+        <v>4996.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>